<commit_message>
update to save progress
</commit_message>
<xml_diff>
--- a/TESTING/legendre_out/DATA/p1/p1FitPoints.xlsx
+++ b/TESTING/legendre_out/DATA/p1/p1FitPoints.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F229"/>
+  <dimension ref="A1:D229"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -382,16 +382,6 @@
           <t>fitOrder</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>splineX</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>splineY</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -408,12 +398,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E2" t="n">
-        <v>3.424536350759639</v>
-      </c>
-      <c r="F2" t="n">
-        <v>2.726124342772388e-05</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -430,12 +414,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E3" t="n">
-        <v>3.42877843536789</v>
-      </c>
-      <c r="F3" t="n">
-        <v>4.935353810599743e-05</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -452,12 +430,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E4" t="n">
-        <v>3.430466699343294</v>
-      </c>
-      <c r="F4" t="n">
-        <v>5.48462261798597e-05</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -474,12 +446,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E5" t="n">
-        <v>3.432206382526072</v>
-      </c>
-      <c r="F5" t="n">
-        <v>7.207035304591853e-05</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -496,12 +462,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E6" t="n">
-        <v>3.433920356105163</v>
-      </c>
-      <c r="F6" t="n">
-        <v>8.165364361349431e-05</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -518,12 +478,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E7" t="n">
-        <v>3.435737168099</v>
-      </c>
-      <c r="F7" t="n">
-        <v>7.708894480819242e-05</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -540,12 +494,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E8" t="n">
-        <v>3.436542735681173</v>
-      </c>
-      <c r="F8" t="n">
-        <v>8.779946831763992e-05</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -562,12 +510,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E9" t="n">
-        <v>3.440861949100481</v>
-      </c>
-      <c r="F9" t="n">
-        <v>7.846171708588319e-05</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -584,12 +526,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E10" t="n">
-        <v>3.444324175730245</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.0001085652582031373</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -606,12 +542,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E11" t="n">
-        <v>3.445018335029777</v>
-      </c>
-      <c r="F11" t="n">
-        <v>8.245536119676371e-05</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -628,12 +558,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E12" t="n">
-        <v>3.44940610739225</v>
-      </c>
-      <c r="F12" t="n">
-        <v>9.923782598740972e-05</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -650,12 +574,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E13" t="n">
-        <v>3.453639622132605</v>
-      </c>
-      <c r="F13" t="n">
-        <v>9.502532551466234e-05</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -672,12 +590,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E14" t="n">
-        <v>3.45806167396666</v>
-      </c>
-      <c r="F14" t="n">
-        <v>7.684244950481798e-05</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -694,12 +606,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E15" t="n">
-        <v>3.659299311887736</v>
-      </c>
-      <c r="F15" t="n">
-        <v>0.0001201543548475927</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -716,12 +622,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E16" t="n">
-        <v>3.676516176489705</v>
-      </c>
-      <c r="F16" t="n">
-        <v>0.0001067692742660575</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -738,12 +638,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E17" t="n">
-        <v>3.677433152354519</v>
-      </c>
-      <c r="F17" t="n">
-        <v>9.155409903455543e-05</v>
-      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -760,12 +654,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E18" t="n">
-        <v>3.679207115008878</v>
-      </c>
-      <c r="F18" t="n">
-        <v>0.0001013073622960785</v>
-      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -782,12 +670,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E19" t="n">
-        <v>3.680072671666319</v>
-      </c>
-      <c r="F19" t="n">
-        <v>8.455744936512585e-05</v>
-      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -804,12 +686,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E20" t="n">
-        <v>3.680886809116387</v>
-      </c>
-      <c r="F20" t="n">
-        <v>0.000105283202110569</v>
-      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -826,12 +702,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E21" t="n">
-        <v>3.681743795905933</v>
-      </c>
-      <c r="F21" t="n">
-        <v>9.52177198546456e-05</v>
-      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -848,12 +718,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E22" t="n">
-        <v>3.682660771770746</v>
-      </c>
-      <c r="F22" t="n">
-        <v>0.0001034173385704508</v>
-      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -870,12 +734,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E23" t="n">
-        <v>3.683397780409756</v>
-      </c>
-      <c r="F23" t="n">
-        <v>0.0001882088570395634</v>
-      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -892,12 +750,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E24" t="n">
-        <v>3.684263337067197</v>
-      </c>
-      <c r="F24" t="n">
-        <v>0.0001965816917958952</v>
-      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -914,12 +766,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E25" t="n">
-        <v>3.685943031174706</v>
-      </c>
-      <c r="F25" t="n">
-        <v>0.0003794569286781079</v>
-      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -936,12 +782,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E26" t="n">
-        <v>3.687699854093274</v>
-      </c>
-      <c r="F26" t="n">
-        <v>0.0003408269510722321</v>
-      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -958,12 +798,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E27" t="n">
-        <v>3.689525235955006</v>
-      </c>
-      <c r="F27" t="n">
-        <v>0.000367647972830256</v>
-      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -980,12 +814,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E28" t="n">
-        <v>3.691256349269888</v>
-      </c>
-      <c r="F28" t="n">
-        <v>0.0003550032804761017</v>
-      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -1002,12 +830,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E29" t="n">
-        <v>3.693013172188456</v>
-      </c>
-      <c r="F29" t="n">
-        <v>0.0003664659288509281</v>
-      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -1024,12 +846,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E30" t="n">
-        <v>3.693578783469556</v>
-      </c>
-      <c r="F30" t="n">
-        <v>0.0003708886814185478</v>
-      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -1046,12 +862,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E31" t="n">
-        <v>3.694615737484906</v>
-      </c>
-      <c r="F31" t="n">
-        <v>0.0003058352886890334</v>
-      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -1068,12 +878,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E32" t="n">
-        <v>3.696278291856625</v>
-      </c>
-      <c r="F32" t="n">
-        <v>0.0003045411789227117</v>
-      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -1090,12 +894,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E33" t="n">
-        <v>3.698009405171506</v>
-      </c>
-      <c r="F33" t="n">
-        <v>0.0003387572479725098</v>
-      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -1112,12 +910,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E34" t="n">
-        <v>3.699783367825865</v>
-      </c>
-      <c r="F34" t="n">
-        <v>0.0003302723275735678</v>
-      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -1134,12 +926,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E35" t="n">
-        <v>3.70147163180127</v>
-      </c>
-      <c r="F35" t="n">
-        <v>0.0003639678227879325</v>
-      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -1156,12 +942,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E36" t="n">
-        <v>3.703177035512466</v>
-      </c>
-      <c r="F36" t="n">
-        <v>0.0003309302016845045</v>
-      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -1178,12 +958,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E37" t="n">
-        <v>3.704736751469439</v>
-      </c>
-      <c r="F37" t="n">
-        <v>0.0003164759091873669</v>
-      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -1200,12 +974,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E38" t="n">
-        <v>3.706647832010125</v>
-      </c>
-      <c r="F38" t="n">
-        <v>0.0002496146576996743</v>
-      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -1222,12 +990,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E39" t="n">
-        <v>3.708276106910262</v>
-      </c>
-      <c r="F39" t="n">
-        <v>0.000245033832940427</v>
-      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -1244,12 +1006,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E40" t="n">
-        <v>3.709964370885666</v>
-      </c>
-      <c r="F40" t="n">
-        <v>0.000197090184118567</v>
-      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -1266,12 +1022,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E41" t="n">
-        <v>3.710855637146794</v>
-      </c>
-      <c r="F41" t="n">
-        <v>0.0002124435365627839</v>
-      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -1288,12 +1038,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E42" t="n">
-        <v>3.711772613011608</v>
-      </c>
-      <c r="F42" t="n">
-        <v>0.0003183694769068522</v>
-      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -1310,12 +1054,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E43" t="n">
-        <v>3.713529435930176</v>
-      </c>
-      <c r="F43" t="n">
-        <v>0.0003212363534048611</v>
-      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -1332,12 +1070,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E44" t="n">
-        <v>3.715166280698207</v>
-      </c>
-      <c r="F44" t="n">
-        <v>0.0003117864731279345</v>
-      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -1354,12 +1086,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E45" t="n">
-        <v>3.719356946099085</v>
-      </c>
-      <c r="F45" t="n">
-        <v>0.0002812897249755586</v>
-      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -1376,12 +1102,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E46" t="n">
-        <v>3.723504762160485</v>
-      </c>
-      <c r="F46" t="n">
-        <v>0.0002888041406164193</v>
-      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -1398,12 +1118,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E47" t="n">
-        <v>3.727875394787168</v>
-      </c>
-      <c r="F47" t="n">
-        <v>0.0002793590200155659</v>
-      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -1420,12 +1134,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E48" t="n">
-        <v>3.745075119653346</v>
-      </c>
-      <c r="F48" t="n">
-        <v>0.000194072597133356</v>
-      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -1442,12 +1150,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E49" t="n">
-        <v>3.762300554123211</v>
-      </c>
-      <c r="F49" t="n">
-        <v>0.0002555010899220769</v>
-      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -1464,12 +1166,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E50" t="n">
-        <v>3.779337451499375</v>
-      </c>
-      <c r="F50" t="n">
-        <v>0.0003805244266248611</v>
-      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -1486,12 +1182,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E51" t="n">
-        <v>3.788087286620635</v>
-      </c>
-      <c r="F51" t="n">
-        <v>0.0005587776917435288</v>
-      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -1508,12 +1198,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E52" t="n">
-        <v>3.796605735308717</v>
-      </c>
-      <c r="F52" t="n">
-        <v>0.0007700655418218724</v>
-      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -1530,12 +1214,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E53" t="n">
-        <v>3.805055625053636</v>
-      </c>
-      <c r="F53" t="n">
-        <v>0.001587918133699719</v>
-      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -1552,12 +1230,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E54" t="n">
-        <v>3.813539794270136</v>
-      </c>
-      <c r="F54" t="n">
-        <v>0.002742303918094362</v>
-      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -1574,12 +1246,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E55" t="n">
-        <v>3.817867577557342</v>
-      </c>
-      <c r="F55" t="n">
-        <v>0.007447663932935442</v>
-      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -1596,12 +1262,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E56" t="n">
-        <v>3.82226391978771</v>
-      </c>
-      <c r="F56" t="n">
-        <v>0.01204216733567591</v>
-      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -1618,12 +1278,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E57" t="n">
-        <v>3.830696669796837</v>
-      </c>
-      <c r="F57" t="n">
-        <v>0.01336037161928329</v>
-      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -1640,12 +1294,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E58" t="n">
-        <v>3.837569703848993</v>
-      </c>
-      <c r="F58" t="n">
-        <v>0.01076930641131473</v>
-      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -1662,12 +1310,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E59" t="n">
-        <v>3.844554146183789</v>
-      </c>
-      <c r="F59" t="n">
-        <v>0.005548407335299294</v>
-      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -1684,12 +1326,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E60" t="n">
-        <v>3.846319538970252</v>
-      </c>
-      <c r="F60" t="n">
-        <v>0.004278512678558955</v>
-      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -1706,12 +1342,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E61" t="n">
-        <v>3.847930674134597</v>
-      </c>
-      <c r="F61" t="n">
-        <v>0.005421204231184439</v>
-      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -1728,12 +1358,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E62" t="n">
-        <v>3.84977319573212</v>
-      </c>
-      <c r="F62" t="n">
-        <v>0.002398731271156932</v>
-      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -1750,12 +1374,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E63" t="n">
-        <v>3.852147049139162</v>
-      </c>
-      <c r="F63" t="n">
-        <v>0.001720684644726185</v>
-      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -1772,12 +1390,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E64" t="n">
-        <v>3.856414843351097</v>
-      </c>
-      <c r="F64" t="n">
-        <v>0.0009932611480053441</v>
-      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -1794,12 +1406,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E65" t="n">
-        <v>3.865190388076044</v>
-      </c>
-      <c r="F65" t="n">
-        <v>0.0005318750025434704</v>
-      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -1816,12 +1422,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E66" t="n">
-        <v>3.866878652051449</v>
-      </c>
-      <c r="F66" t="n">
-        <v>0.0004070454453229111</v>
-      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -1838,12 +1438,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E67" t="n">
-        <v>3.869363913741131</v>
-      </c>
-      <c r="F67" t="n">
-        <v>0.000397932677226525</v>
-      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -1860,12 +1454,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E68" t="n">
-        <v>3.873640277820963</v>
-      </c>
-      <c r="F68" t="n">
-        <v>0.0004832463289749285</v>
-      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -1882,12 +1470,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E69" t="n">
-        <v>3.878070899522913</v>
-      </c>
-      <c r="F69" t="n">
-        <v>0.0006696065287930627</v>
-      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -1904,12 +1486,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E70" t="n">
-        <v>3.881644534435317</v>
-      </c>
-      <c r="F70" t="n">
-        <v>0.0006239025709367391</v>
-      </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
@@ -1926,12 +1502,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E71" t="n">
-        <v>3.88648650979625</v>
-      </c>
-      <c r="F71" t="n">
-        <v>0.001249176154741283</v>
-      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -1948,12 +1518,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E72" t="n">
-        <v>3.890925701366096</v>
-      </c>
-      <c r="F72" t="n">
-        <v>0.001893940938944161</v>
-      </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -1970,12 +1534,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E73" t="n">
-        <v>3.899118495074151</v>
-      </c>
-      <c r="F73" t="n">
-        <v>0.004759079781038328</v>
-      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -1992,12 +1550,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E74" t="n">
-        <v>3.908014017949633</v>
-      </c>
-      <c r="F74" t="n">
-        <v>0.01210333671197988</v>
-      </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -2014,12 +1566,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E75" t="n">
-        <v>3.916541036505611</v>
-      </c>
-      <c r="F75" t="n">
-        <v>0.01199326791716576</v>
-      </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
@@ -2036,12 +1582,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E76" t="n">
-        <v>3.925025205722112</v>
-      </c>
-      <c r="F76" t="n">
-        <v>0.00649488550990609</v>
-      </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
@@ -2058,12 +1598,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E77" t="n">
-        <v>3.933637922957044</v>
-      </c>
-      <c r="F77" t="n">
-        <v>0.003438892302487163</v>
-      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
@@ -2080,12 +1614,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E78" t="n">
-        <v>3.942370618342513</v>
-      </c>
-      <c r="F78" t="n">
-        <v>0.001708285988755101</v>
-      </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
@@ -2102,12 +1630,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E79" t="n">
-        <v>3.950700529936895</v>
-      </c>
-      <c r="F79" t="n">
-        <v>0.00173520832058068</v>
-      </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
@@ -2124,12 +1646,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E80" t="n">
-        <v>3.959476074661841</v>
-      </c>
-      <c r="F80" t="n">
-        <v>0.001152515929054183</v>
-      </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
@@ -2146,12 +1662,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E81" t="n">
-        <v>3.967797416388328</v>
-      </c>
-      <c r="F81" t="n">
-        <v>0.001103231158833114</v>
-      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
@@ -2168,12 +1678,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E82" t="n">
-        <v>3.97227945729765</v>
-      </c>
-      <c r="F82" t="n">
-        <v>0.0006665025254806228</v>
-      </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
@@ -2190,12 +1694,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E83" t="n">
-        <v>3.976384424019573</v>
-      </c>
-      <c r="F83" t="n">
-        <v>0.0008092212748635805</v>
-      </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
@@ -2212,12 +1710,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E84" t="n">
-        <v>3.984954291915029</v>
-      </c>
-      <c r="F84" t="n">
-        <v>0.001738141210423208</v>
-      </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
@@ -2234,12 +1726,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E85" t="n">
-        <v>4.002231145592266</v>
-      </c>
-      <c r="F85" t="n">
-        <v>0.001165547357243525</v>
-      </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
@@ -2256,12 +1742,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E86" t="n">
-        <v>4.010826723091408</v>
-      </c>
-      <c r="F86" t="n">
-        <v>0.0005315440266260533</v>
-      </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
@@ -2278,12 +1758,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E87" t="n">
-        <v>4.019208053893163</v>
-      </c>
-      <c r="F87" t="n">
-        <v>0.0004528179708796148</v>
-      </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
@@ -2300,12 +1774,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E88" t="n">
-        <v>4.036424918495132</v>
-      </c>
-      <c r="F88" t="n">
-        <v>0.0004192715499912967</v>
-      </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
@@ -2322,12 +1790,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E89" t="n">
-        <v>4.053547514550251</v>
-      </c>
-      <c r="F89" t="n">
-        <v>0.0005317727979734225</v>
-      </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
@@ -2344,12 +1806,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E90" t="n">
-        <v>4.070687250341162</v>
-      </c>
-      <c r="F90" t="n">
-        <v>0.0009713367875781591</v>
-      </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
@@ -2366,12 +1822,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E91" t="n">
-        <v>4.075126441911007</v>
-      </c>
-      <c r="F91" t="n">
-        <v>0.002227065407970377</v>
-      </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
@@ -2388,12 +1838,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E92" t="n">
-        <v>4.078297293032326</v>
-      </c>
-      <c r="F92" t="n">
-        <v>0.002510381599109668</v>
-      </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
@@ -2410,12 +1854,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E93" t="n">
-        <v>4.087861265603653</v>
-      </c>
-      <c r="F93" t="n">
-        <v>0.002945197325218724</v>
-      </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
@@ -2432,12 +1870,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E94" t="n">
-        <v>4.09212905981559</v>
-      </c>
-      <c r="F94" t="n">
-        <v>0.003049178821473336</v>
-      </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
@@ -2454,12 +1886,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E95" t="n">
-        <v>4.096551111649645</v>
-      </c>
-      <c r="F95" t="n">
-        <v>0.002718295693181587</v>
-      </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
@@ -2476,12 +1902,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E96" t="n">
-        <v>4.105069560337727</v>
-      </c>
-      <c r="F96" t="n">
-        <v>0.002366069596782138</v>
-      </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
@@ -2498,12 +1918,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E97" t="n">
-        <v>4.113468030875272</v>
-      </c>
-      <c r="F97" t="n">
-        <v>0.001793160797384424</v>
-      </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
@@ -2520,12 +1934,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E98" t="n">
-        <v>4.122132167317578</v>
-      </c>
-      <c r="F98" t="n">
-        <v>0.00166139834064013</v>
-      </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
@@ -2542,12 +1950,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E99" t="n">
-        <v>4.12395754917931</v>
-      </c>
-      <c r="F99" t="n">
-        <v>0.001559987167849485</v>
-      </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
@@ -2564,12 +1966,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E100" t="n">
-        <v>4.126622778094797</v>
-      </c>
-      <c r="F100" t="n">
-        <v>0.00153303016251472</v>
-      </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
@@ -2586,12 +1982,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E101" t="n">
-        <v>4.13072774481672</v>
-      </c>
-      <c r="F101" t="n">
-        <v>0.001515455165276498</v>
-      </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
@@ -2608,12 +1998,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E102" t="n">
-        <v>4.139151924957952</v>
-      </c>
-      <c r="F102" t="n">
-        <v>0.001520660309484841</v>
-      </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
@@ -2630,12 +2014,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E103" t="n">
-        <v>4.156411638899399</v>
-      </c>
-      <c r="F103" t="n">
-        <v>0.001791690207407932</v>
-      </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
@@ -2652,12 +2030,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E104" t="n">
-        <v>4.170346244097408</v>
-      </c>
-      <c r="F104" t="n">
-        <v>0.002390044210642019</v>
-      </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
@@ -2674,12 +2046,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E105" t="n">
-        <v>4.190571132330683</v>
-      </c>
-      <c r="F105" t="n">
-        <v>0.003910720913537869</v>
-      </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
@@ -2696,12 +2062,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E106" t="n">
-        <v>4.199158139961929</v>
-      </c>
-      <c r="F106" t="n">
-        <v>0.005982000321012501</v>
-      </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
@@ -2718,12 +2078,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E107" t="n">
-        <v>4.207916544951084</v>
-      </c>
-      <c r="F107" t="n">
-        <v>0.007917784675238911</v>
-      </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
@@ -2740,12 +2094,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E108" t="n">
-        <v>4.216340725092316</v>
-      </c>
-      <c r="F108" t="n">
-        <v>0.01053686304886661</v>
-      </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
@@ -2762,12 +2110,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E109" t="n">
-        <v>4.221645473319603</v>
-      </c>
-      <c r="F109" t="n">
-        <v>0.01312394285024387</v>
-      </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
@@ -2784,12 +2126,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E110" t="n">
-        <v>4.225107699949367</v>
-      </c>
-      <c r="F110" t="n">
-        <v>0.01419158366602055</v>
-      </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
@@ -2806,12 +2142,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E111" t="n">
-        <v>4.230875221043007</v>
-      </c>
-      <c r="F111" t="n">
-        <v>0.01770251225619758</v>
-      </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
@@ -2828,12 +2158,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E112" t="n">
-        <v>4.23929940118424</v>
-      </c>
-      <c r="F112" t="n">
-        <v>0.02171504322580034</v>
-      </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
@@ -2850,12 +2174,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E113" t="n">
-        <v>4.24231599468344</v>
-      </c>
-      <c r="F113" t="n">
-        <v>0.02196126986645404</v>
-      </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
@@ -2872,12 +2190,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E114" t="n">
-        <v>4.24787783894759</v>
-      </c>
-      <c r="F114" t="n">
-        <v>0.02463352873431351</v>
-      </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
@@ -2894,12 +2206,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E115" t="n">
-        <v>4.252257041442167</v>
-      </c>
-      <c r="F115" t="n">
-        <v>0.02515885371503485</v>
-      </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
@@ -2916,12 +2222,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E116" t="n">
-        <v>4.25472516339606</v>
-      </c>
-      <c r="F116" t="n">
-        <v>0.02500044238693442</v>
-      </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
@@ -2938,12 +2238,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E117" t="n">
-        <v>4.25739896217944</v>
-      </c>
-      <c r="F117" t="n">
-        <v>0.02458655925439199</v>
-      </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
@@ -2960,12 +2254,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E118" t="n">
-        <v>4.259258623512755</v>
-      </c>
-      <c r="F118" t="n">
-        <v>0.02458202856145001</v>
-      </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
@@ -2982,12 +2270,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E119" t="n">
-        <v>4.2616239070519</v>
-      </c>
-      <c r="F119" t="n">
-        <v>0.0233521290241238</v>
-      </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
@@ -3004,12 +2286,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E120" t="n">
-        <v>4.263192192876769</v>
-      </c>
-      <c r="F120" t="n">
-        <v>0.02279078023761039</v>
-      </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
@@ -3026,12 +2302,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E121" t="n">
-        <v>4.271830619715387</v>
-      </c>
-      <c r="F121" t="n">
-        <v>0.01873548822528431</v>
-      </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
@@ -3048,12 +2318,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E122" t="n">
-        <v>4.27642406890735</v>
-      </c>
-      <c r="F122" t="n">
-        <v>0.01740379581136126</v>
-      </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
@@ -3070,12 +2334,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E123" t="n">
-        <v>4.28036620813926</v>
-      </c>
-      <c r="F123" t="n">
-        <v>0.01465431828368129</v>
-      </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
@@ -3092,12 +2350,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E124" t="n">
-        <v>4.28891036643103</v>
-      </c>
-      <c r="F124" t="n">
-        <v>0.01138183767303974</v>
-      </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
@@ -3114,12 +2366,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E125" t="n">
-        <v>4.293495245755098</v>
-      </c>
-      <c r="F125" t="n">
-        <v>0.01039181684647338</v>
-      </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
@@ -3136,12 +2382,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E126" t="n">
-        <v>4.297651631684394</v>
-      </c>
-      <c r="F126" t="n">
-        <v>0.008958789382230685</v>
-      </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
@@ -3158,12 +2398,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E127" t="n">
-        <v>4.300136893374075</v>
-      </c>
-      <c r="F127" t="n">
-        <v>0.008529125761831256</v>
-      </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
@@ -3180,12 +2414,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E128" t="n">
-        <v>4.300239731788821</v>
-      </c>
-      <c r="F128" t="n">
-        <v>0.008566972435572797</v>
-      </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="n">
@@ -3202,12 +2430,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E129" t="n">
-        <v>4.30191942589633</v>
-      </c>
-      <c r="F129" t="n">
-        <v>0.00847558534834251</v>
-      </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
@@ -3224,12 +2446,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E130" t="n">
-        <v>4.306187220108267</v>
-      </c>
-      <c r="F130" t="n">
-        <v>0.008227157939632999</v>
-      </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="n">
@@ -3246,12 +2462,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E131" t="n">
-        <v>4.308783890080591</v>
-      </c>
-      <c r="F131" t="n">
-        <v>0.008282159021159433</v>
-      </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="n">
@@ -3268,12 +2478,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E132" t="n">
-        <v>4.310729250092858</v>
-      </c>
-      <c r="F132" t="n">
-        <v>0.008392153858361033</v>
-      </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
@@ -3290,12 +2494,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E133" t="n">
-        <v>4.31302597468884</v>
-      </c>
-      <c r="F133" t="n">
-        <v>0.009323082227477398</v>
-      </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="n">
@@ -3312,12 +2510,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E134" t="n">
-        <v>4.315699773472222</v>
-      </c>
-      <c r="F134" t="n">
-        <v>0.01019256361101952</v>
-      </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="n">
@@ -3334,12 +2526,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E135" t="n">
-        <v>4.318107906350845</v>
-      </c>
-      <c r="F135" t="n">
-        <v>0.01068827426623893</v>
-      </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="n">
@@ -3356,12 +2542,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E136" t="n">
-        <v>4.320910253152659</v>
-      </c>
-      <c r="F136" t="n">
-        <v>0.01084733066380565</v>
-      </c>
     </row>
     <row r="137">
       <c r="A137" s="1" t="n">
@@ -3378,12 +2558,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E137" t="n">
-        <v>4.323318386031281</v>
-      </c>
-      <c r="F137" t="n">
-        <v>0.01059276760250125</v>
-      </c>
     </row>
     <row r="138">
       <c r="A138" s="1" t="n">
@@ -3400,12 +2574,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E138" t="n">
-        <v>4.327757577601127</v>
-      </c>
-      <c r="F138" t="n">
-        <v>0.01005086227455396</v>
-      </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="n">
@@ -3422,12 +2590,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E139" t="n">
-        <v>4.331931103266214</v>
-      </c>
-      <c r="F139" t="n">
-        <v>0.008670632493768133</v>
-      </c>
     </row>
     <row r="140">
       <c r="A140" s="1" t="n">
@@ -3444,12 +2606,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E140" t="n">
-        <v>4.340535250633251</v>
-      </c>
-      <c r="F140" t="n">
-        <v>0.005413111066881513</v>
-      </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="n">
@@ -3466,12 +2622,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E141" t="n">
-        <v>4.344845894184665</v>
-      </c>
-      <c r="F141" t="n">
-        <v>0.004542435013471957</v>
-      </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="n">
@@ -3488,12 +2638,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E142" t="n">
-        <v>4.348762323812888</v>
-      </c>
-      <c r="F142" t="n">
-        <v>0.003663309281463038</v>
-      </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="n">
@@ -3510,12 +2654,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E143" t="n">
-        <v>4.357083665539375</v>
-      </c>
-      <c r="F143" t="n">
-        <v>0.002826518959901516</v>
-      </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="n">
@@ -3532,12 +2670,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E144" t="n">
-        <v>4.362054188918739</v>
-      </c>
-      <c r="F144" t="n">
-        <v>0.002671616505545902</v>
-      </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="n">
@@ -3554,12 +2686,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E145" t="n">
-        <v>4.365250749643743</v>
-      </c>
-      <c r="F145" t="n">
-        <v>0.002578686207869555</v>
-      </c>
     </row>
     <row r="146">
       <c r="A146" s="1" t="n">
@@ -3576,12 +2702,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E146" t="n">
-        <v>4.367855989483961</v>
-      </c>
-      <c r="F146" t="n">
-        <v>0.002685455272876407</v>
-      </c>
     </row>
     <row r="147">
       <c r="A147" s="1" t="n">
@@ -3598,12 +2718,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E147" t="n">
-        <v>4.369681371345694</v>
-      </c>
-      <c r="F147" t="n">
-        <v>0.002546685145449765</v>
-      </c>
     </row>
     <row r="148">
       <c r="A148" s="1" t="n">
@@ -3620,12 +2734,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E148" t="n">
-        <v>4.370624056814194</v>
-      </c>
-      <c r="F148" t="n">
-        <v>0.002541033888203071</v>
-      </c>
     </row>
     <row r="149">
       <c r="A149" s="1" t="n">
@@ -3642,12 +2750,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E149" t="n">
-        <v>4.371001131001594</v>
-      </c>
-      <c r="F149" t="n">
-        <v>0.002543219297378939</v>
-      </c>
     </row>
     <row r="150">
       <c r="A150" s="1" t="n">
@@ -3664,12 +2766,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E150" t="n">
-        <v>4.371241087302666</v>
-      </c>
-      <c r="F150" t="n">
-        <v>0.002502555026460214</v>
-      </c>
     </row>
     <row r="151">
       <c r="A151" s="1" t="n">
@@ -3686,12 +2782,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E151" t="n">
-        <v>4.37310074863598</v>
-      </c>
-      <c r="F151" t="n">
-        <v>0.002506838829053667</v>
-      </c>
     </row>
     <row r="152">
       <c r="A152" s="1" t="n">
@@ -3708,12 +2798,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E152" t="n">
-        <v>4.37479758247928</v>
-      </c>
-      <c r="F152" t="n">
-        <v>0.002422304860484723</v>
-      </c>
     </row>
     <row r="153">
       <c r="A153" s="1" t="n">
@@ -3730,12 +2814,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E153" t="n">
-        <v>4.376545835529954</v>
-      </c>
-      <c r="F153" t="n">
-        <v>0.002408493402906308</v>
-      </c>
     </row>
     <row r="154">
       <c r="A154" s="1" t="n">
@@ -3752,12 +2830,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E154" t="n">
-        <v>4.378156970694299</v>
-      </c>
-      <c r="F154" t="n">
-        <v>0.002231763230024475</v>
-      </c>
     </row>
     <row r="155">
       <c r="A155" s="1" t="n">
@@ -3774,12 +2846,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E155" t="n">
-        <v>4.379236774049127</v>
-      </c>
-      <c r="F155" t="n">
-        <v>0.002247240282045541</v>
-      </c>
     </row>
     <row r="156">
       <c r="A156" s="1" t="n">
@@ -3796,12 +2862,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E156" t="n">
-        <v>4.379845234669704</v>
-      </c>
-      <c r="F156" t="n">
-        <v>0.002274303286269798</v>
-      </c>
     </row>
     <row r="157">
       <c r="A157" s="1" t="n">
@@ -3818,12 +2878,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E157" t="n">
-        <v>4.382493323849399</v>
-      </c>
-      <c r="F157" t="n">
-        <v>0.002259640671839816</v>
-      </c>
     </row>
     <row r="158">
       <c r="A158" s="1" t="n">
@@ -3840,12 +2894,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E158" t="n">
-        <v>4.386743978325545</v>
-      </c>
-      <c r="F158" t="n">
-        <v>0.001994252349826539</v>
-      </c>
     </row>
     <row r="159">
       <c r="A159" s="1" t="n">
@@ -3862,12 +2910,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E159" t="n">
-        <v>4.391003202669586</v>
-      </c>
-      <c r="F159" t="n">
-        <v>0.001748408901966254</v>
-      </c>
     </row>
     <row r="160">
       <c r="A160" s="1" t="n">
@@ -3884,12 +2926,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E160" t="n">
-        <v>4.395073889919927</v>
-      </c>
-      <c r="F160" t="n">
-        <v>0.001624323818029944</v>
-      </c>
     </row>
     <row r="161">
       <c r="A161" s="1" t="n">
@@ -3906,12 +2942,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E161" t="n">
-        <v>4.396290811161082</v>
-      </c>
-      <c r="F161" t="n">
-        <v>0.001588555302355699</v>
-      </c>
     </row>
     <row r="162">
       <c r="A162" s="1" t="n">
@@ -3928,12 +2958,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E162" t="n">
-        <v>4.399607350036622</v>
-      </c>
-      <c r="F162" t="n">
-        <v>0.001994636125800829</v>
-      </c>
     </row>
     <row r="163">
       <c r="A163" s="1" t="n">
@@ -3950,12 +2974,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E163" t="n">
-        <v>4.403952273059619</v>
-      </c>
-      <c r="F163" t="n">
-        <v>0.003472011792322736</v>
-      </c>
     </row>
     <row r="164">
       <c r="A164" s="1" t="n">
@@ -3972,12 +2990,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E164" t="n">
-        <v>4.406326126466659</v>
-      </c>
-      <c r="F164" t="n">
-        <v>0.004208052579934978</v>
-      </c>
     </row>
     <row r="165">
       <c r="A165" s="1" t="n">
@@ -3994,12 +3006,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E165" t="n">
-        <v>4.408974215646356</v>
-      </c>
-      <c r="F165" t="n">
-        <v>0.004479891072399068</v>
-      </c>
     </row>
     <row r="166">
       <c r="A166" s="1" t="n">
@@ -4016,12 +3022,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E166" t="n">
-        <v>4.411759422712378</v>
-      </c>
-      <c r="F166" t="n">
-        <v>0.004553401872913912</v>
-      </c>
     </row>
     <row r="167">
       <c r="A167" s="1" t="n">
@@ -4038,12 +3038,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E167" t="n">
-        <v>4.41349053602726</v>
-      </c>
-      <c r="F167" t="n">
-        <v>0.004669988074459768</v>
-      </c>
     </row>
     <row r="168">
       <c r="A168" s="1" t="n">
@@ -4060,12 +3054,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E168" t="n">
-        <v>4.414321813213119</v>
-      </c>
-      <c r="F168" t="n">
-        <v>0.004741510573049734</v>
-      </c>
     </row>
     <row r="169">
       <c r="A169" s="1" t="n">
@@ -4082,12 +3070,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E169" t="n">
-        <v>4.419515153157765</v>
-      </c>
-      <c r="F169" t="n">
-        <v>0.004558754816660753</v>
-      </c>
     </row>
     <row r="170">
       <c r="A170" s="1" t="n">
@@ -4104,12 +3086,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E170" t="n">
-        <v>4.421511932377406</v>
-      </c>
-      <c r="F170" t="n">
-        <v>0.004200870025133713</v>
-      </c>
     </row>
     <row r="171">
       <c r="A171" s="1" t="n">
@@ -4126,12 +3102,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E171" t="n">
-        <v>4.430664551289752</v>
-      </c>
-      <c r="F171" t="n">
-        <v>0.002637176627311947</v>
-      </c>
     </row>
     <row r="172">
       <c r="A172" s="1" t="n">
@@ -4148,12 +3118,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E172" t="n">
-        <v>4.447624319854858</v>
-      </c>
-      <c r="F172" t="n">
-        <v>0.001718998822072707</v>
-      </c>
     </row>
     <row r="173">
       <c r="A173" s="1" t="n">
@@ -4170,12 +3134,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E173" t="n">
-        <v>4.464926883135782</v>
-      </c>
-      <c r="F173" t="n">
-        <v>0.001577684032826449</v>
-      </c>
     </row>
     <row r="174">
       <c r="A174" s="1" t="n">
@@ -4192,12 +3150,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E174" t="n">
-        <v>4.482066618926692</v>
-      </c>
-      <c r="F174" t="n">
-        <v>0.001824572920525541</v>
-      </c>
     </row>
     <row r="175">
       <c r="A175" s="1" t="n">
@@ -4214,12 +3166,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E175" t="n">
-        <v>4.490182283823687</v>
-      </c>
-      <c r="F175" t="n">
-        <v>0.002555534019728641</v>
-      </c>
     </row>
     <row r="176">
       <c r="A176" s="1" t="n">
@@ -4236,12 +3182,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E176" t="n">
-        <v>4.493233156794469</v>
-      </c>
-      <c r="F176" t="n">
-        <v>0.002827532230629263</v>
-      </c>
     </row>
     <row r="177">
       <c r="A177" s="1" t="n">
@@ -4258,12 +3198,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E177" t="n">
-        <v>4.499292053396556</v>
-      </c>
-      <c r="F177" t="n">
-        <v>0.004295466416294982</v>
-      </c>
     </row>
     <row r="178">
       <c r="A178" s="1" t="n">
@@ -4280,12 +3214,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E178" t="n">
-        <v>4.507699093801998</v>
-      </c>
-      <c r="F178" t="n">
-        <v>0.005788356242966136</v>
-      </c>
     </row>
     <row r="179">
       <c r="A179" s="1" t="n">
@@ -4302,12 +3230,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E179" t="n">
-        <v>4.512069726428679</v>
-      </c>
-      <c r="F179" t="n">
-        <v>0.00604343557355911</v>
-      </c>
     </row>
     <row r="180">
       <c r="A180" s="1" t="n">
@@ -4324,12 +3246,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E180" t="n">
-        <v>4.516303241169035</v>
-      </c>
-      <c r="F180" t="n">
-        <v>0.005757471640857811</v>
-      </c>
     </row>
     <row r="181">
       <c r="A181" s="1" t="n">
@@ -4346,12 +3262,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E181" t="n">
-        <v>4.520571035380971</v>
-      </c>
-      <c r="F181" t="n">
-        <v>0.00514481147108176</v>
-      </c>
     </row>
     <row r="182">
       <c r="A182" s="1" t="n">
@@ -4368,12 +3278,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E182" t="n">
-        <v>4.520622454588343</v>
-      </c>
-      <c r="F182" t="n">
-        <v>0.005178640025432485</v>
-      </c>
     </row>
     <row r="183">
       <c r="A183" s="1" t="n">
@@ -4390,12 +3294,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E183" t="n">
-        <v>4.524727421310266</v>
-      </c>
-      <c r="F183" t="n">
-        <v>0.004590587219246101</v>
-      </c>
     </row>
     <row r="184">
       <c r="A184" s="1" t="n">
@@ -4412,12 +3310,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E184" t="n">
-        <v>4.529132333408531</v>
-      </c>
-      <c r="F184" t="n">
-        <v>0.003890814512660001</v>
-      </c>
     </row>
     <row r="185">
       <c r="A185" s="1" t="n">
@@ -4434,12 +3326,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E185" t="n">
-        <v>4.533597234582063</v>
-      </c>
-      <c r="F185" t="n">
-        <v>0.003564821090230182</v>
-      </c>
     </row>
     <row r="186">
       <c r="A186" s="1" t="n">
@@ -4456,12 +3342,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E186" t="n">
-        <v>4.535979657856999</v>
-      </c>
-      <c r="F186" t="n">
-        <v>0.00361836214227122</v>
-      </c>
     </row>
     <row r="187">
       <c r="A187" s="1" t="n">
@@ -4478,12 +3358,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E187" t="n">
-        <v>4.540033205371549</v>
-      </c>
-      <c r="F187" t="n">
-        <v>0.003533767615550085</v>
-      </c>
     </row>
     <row r="188">
       <c r="A188" s="1" t="n">
@@ -4500,12 +3374,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E188" t="n">
-        <v>4.541790028290118</v>
-      </c>
-      <c r="F188" t="n">
-        <v>0.003505908955132054</v>
-      </c>
     </row>
     <row r="189">
       <c r="A189" s="1" t="n">
@@ -4522,12 +3390,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E189" t="n">
-        <v>4.54406961315031</v>
-      </c>
-      <c r="F189" t="n">
-        <v>0.003300374404613294</v>
-      </c>
     </row>
     <row r="190">
       <c r="A190" s="1" t="n">
@@ -4544,12 +3406,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E190" t="n">
-        <v>4.54908298586915</v>
-      </c>
-      <c r="F190" t="n">
-        <v>0.003701281112022689</v>
-      </c>
     </row>
     <row r="191">
       <c r="A191" s="1" t="n">
@@ -4566,12 +3422,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E191" t="n">
-        <v>4.553067974440538</v>
-      </c>
-      <c r="F191" t="n">
-        <v>0.004289219128474648</v>
-      </c>
     </row>
     <row r="192">
       <c r="A192" s="1" t="n">
@@ -4588,12 +3438,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E192" t="n">
-        <v>4.557044393144028</v>
-      </c>
-      <c r="F192" t="n">
-        <v>0.004867398388227901</v>
-      </c>
     </row>
     <row r="193">
       <c r="A193" s="1" t="n">
@@ -4610,12 +3454,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E193" t="n">
-        <v>4.561577853260723</v>
-      </c>
-      <c r="F193" t="n">
-        <v>0.005493722740334901</v>
-      </c>
     </row>
     <row r="194">
       <c r="A194" s="1" t="n">
@@ -4632,12 +3470,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E194" t="n">
-        <v>4.56575137892581</v>
-      </c>
-      <c r="F194" t="n">
-        <v>0.006389248051757859</v>
-      </c>
     </row>
     <row r="195">
       <c r="A195" s="1" t="n">
@@ -4654,12 +3486,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E195" t="n">
-        <v>4.570207710231447</v>
-      </c>
-      <c r="F195" t="n">
-        <v>0.007228852298836397</v>
-      </c>
     </row>
     <row r="196">
       <c r="A196" s="1" t="n">
@@ -4676,12 +3502,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E196" t="n">
-        <v>4.570233419835134</v>
-      </c>
-      <c r="F196" t="n">
-        <v>0.006913581883080291</v>
-      </c>
     </row>
     <row r="197">
       <c r="A197" s="1" t="n">
@@ -4698,12 +3518,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E197" t="n">
-        <v>4.574141279595461</v>
-      </c>
-      <c r="F197" t="n">
-        <v>0.00689047042736839</v>
-      </c>
     </row>
     <row r="198">
       <c r="A198" s="1" t="n">
@@ -4720,12 +3534,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E198" t="n">
-        <v>4.578657599976365</v>
-      </c>
-      <c r="F198" t="n">
-        <v>0.006288257088395448</v>
-      </c>
     </row>
     <row r="199">
       <c r="A199" s="1" t="n">
@@ -4742,12 +3550,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E199" t="n">
-        <v>4.578820427466379</v>
-      </c>
-      <c r="F199" t="n">
-        <v>0.006170047362708217</v>
-      </c>
     </row>
     <row r="200">
       <c r="A200" s="1" t="n">
@@ -4764,12 +3566,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E200" t="n">
-        <v>4.582256944492457</v>
-      </c>
-      <c r="F200" t="n">
-        <v>0.005484667680102053</v>
-      </c>
     </row>
     <row r="201">
       <c r="A201" s="1" t="n">
@@ -4786,12 +3582,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E201" t="n">
-        <v>4.583388167054657</v>
-      </c>
-      <c r="F201" t="n">
-        <v>0.005260477783386923</v>
-      </c>
     </row>
     <row r="202">
       <c r="A202" s="1" t="n">
@@ -4808,12 +3598,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E202" t="n">
-        <v>4.583662402827311</v>
-      </c>
-      <c r="F202" t="n">
-        <v>0.005125294617752422</v>
-      </c>
     </row>
     <row r="203">
       <c r="A203" s="1" t="n">
@@ -4830,12 +3614,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E203" t="n">
-        <v>4.586636146987034</v>
-      </c>
-      <c r="F203" t="n">
-        <v>0.006544913747631335</v>
-      </c>
     </row>
     <row r="204">
       <c r="A204" s="1" t="n">
@@ -4852,12 +3630,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E204" t="n">
-        <v>4.58796447651083</v>
-      </c>
-      <c r="F204" t="n">
-        <v>0.005706229081883014</v>
-      </c>
     </row>
     <row r="205">
       <c r="A205" s="1" t="n">
@@ -4874,12 +3646,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E205" t="n">
-        <v>4.591649519705875</v>
-      </c>
-      <c r="F205" t="n">
-        <v>0.006035283640905923</v>
-      </c>
     </row>
     <row r="206">
       <c r="A206" s="1" t="n">
@@ -4896,12 +3662,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E206" t="n">
-        <v>4.591709508781143</v>
-      </c>
-      <c r="F206" t="n">
-        <v>0.006565389229871577</v>
-      </c>
     </row>
     <row r="207">
       <c r="A207" s="1" t="n">
@@ -4918,12 +3678,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E207" t="n">
-        <v>4.593303504209699</v>
-      </c>
-      <c r="F207" t="n">
-        <v>0.005490966412079285</v>
-      </c>
     </row>
     <row r="208">
       <c r="A208" s="1" t="n">
@@ -4940,12 +3694,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E208" t="n">
-        <v>4.595068896996162</v>
-      </c>
-      <c r="F208" t="n">
-        <v>0.005168575921903385</v>
-      </c>
     </row>
     <row r="209">
       <c r="A209" s="1" t="n">
@@ -4962,12 +3710,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E209" t="n">
-        <v>4.596757160971567</v>
-      </c>
-      <c r="F209" t="n">
-        <v>0.00490669583841991</v>
-      </c>
     </row>
     <row r="210">
       <c r="A210" s="1" t="n">
@@ -4984,12 +3726,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E210" t="n">
-        <v>4.598633962040672</v>
-      </c>
-      <c r="F210" t="n">
-        <v>0.004607914031836065</v>
-      </c>
     </row>
     <row r="211">
       <c r="A211" s="1" t="n">
@@ -5006,12 +3742,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E211" t="n">
-        <v>4.600339365751868</v>
-      </c>
-      <c r="F211" t="n">
-        <v>0.004275587379678715</v>
-      </c>
     </row>
     <row r="212">
       <c r="A212" s="1" t="n">
@@ -5028,12 +3758,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E212" t="n">
-        <v>4.600536472713462</v>
-      </c>
-      <c r="F212" t="n">
-        <v>0.004593449266250404</v>
-      </c>
     </row>
     <row r="213">
       <c r="A213" s="1" t="n">
@@ -5050,12 +3774,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E213" t="n">
-        <v>4.601719114483036</v>
-      </c>
-      <c r="F213" t="n">
-        <v>0.004343336334251765</v>
-      </c>
     </row>
     <row r="214">
       <c r="A214" s="1" t="n">
@@ -5072,12 +3790,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E214" t="n">
-        <v>4.603295970175799</v>
-      </c>
-      <c r="F214" t="n">
-        <v>0.005171257019306179</v>
-      </c>
     </row>
     <row r="215">
       <c r="A215" s="1" t="n">
@@ -5094,12 +3806,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E215" t="n">
-        <v>4.604949954679621</v>
-      </c>
-      <c r="F215" t="n">
-        <v>0.003587806556713504</v>
-      </c>
     </row>
     <row r="216">
       <c r="A216" s="1" t="n">
@@ -5116,12 +3822,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E216" t="n">
-        <v>4.606132596449195</v>
-      </c>
-      <c r="F216" t="n">
-        <v>0.002235111212482969</v>
-      </c>
     </row>
     <row r="217">
       <c r="A217" s="1" t="n">
@@ -5138,12 +3838,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E217" t="n">
-        <v>4.610666056565891</v>
-      </c>
-      <c r="F217" t="n">
-        <v>0.0009182225992723854</v>
-      </c>
     </row>
     <row r="218">
       <c r="A218" s="1" t="n">
@@ -5160,12 +3854,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E218" t="n">
-        <v>4.613091329180303</v>
-      </c>
-      <c r="F218" t="n">
-        <v>0.0005694893594816976</v>
-      </c>
     </row>
     <row r="219">
       <c r="A219" s="1" t="n">
@@ -5182,12 +3870,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E219" t="n">
-        <v>4.613451263631914</v>
-      </c>
-      <c r="F219" t="n">
-        <v>0.0008065838186419792</v>
-      </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="n">
@@ -5204,12 +3886,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E220" t="n">
-        <v>4.613896896762476</v>
-      </c>
-      <c r="F220" t="n">
-        <v>0.0005040582750033011</v>
-      </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="n">
@@ -5226,12 +3902,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E221" t="n">
-        <v>4.615696569020522</v>
-      </c>
-      <c r="F221" t="n">
-        <v>0.0004089019025163319</v>
-      </c>
     </row>
     <row r="222">
       <c r="A222" s="1" t="n">
@@ -5248,12 +3918,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E222" t="n">
-        <v>4.619038817499749</v>
-      </c>
-      <c r="F222" t="n">
-        <v>0.000348496837816131</v>
-      </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="n">
@@ -5270,12 +3934,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E223" t="n">
-        <v>4.621798314962087</v>
-      </c>
-      <c r="F223" t="n">
-        <v>0.0003521446723737503</v>
-      </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="n">
@@ -5292,12 +3950,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E224" t="n">
-        <v>4.630650988498092</v>
-      </c>
-      <c r="F224" t="n">
-        <v>0.0005115075643133328</v>
-      </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="n">
@@ -5314,12 +3966,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E225" t="n">
-        <v>4.639795037542543</v>
-      </c>
-      <c r="F225" t="n">
-        <v>0.0009517998453147267</v>
-      </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="n">
@@ -5336,12 +3982,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E226" t="n">
-        <v>4.64860486173907</v>
-      </c>
-      <c r="F226" t="n">
-        <v>0.001065260528910033</v>
-      </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="n">
@@ -5358,12 +3998,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E227" t="n">
-        <v>4.658074565763548</v>
-      </c>
-      <c r="F227" t="n">
-        <v>0.000938995485324857</v>
-      </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="n">
@@ -5380,12 +4014,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E228" t="n">
-        <v>4.661373964903298</v>
-      </c>
-      <c r="F228" t="n">
-        <v>0.0008352824546536999</v>
-      </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="n">
@@ -5401,12 +4029,6 @@
         <is>
           <t>4</t>
         </is>
-      </c>
-      <c r="E229" t="n">
-        <v>4.662710864294989</v>
-      </c>
-      <c r="F229" t="n">
-        <v>0.0008606171881907121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>